<commit_message>
combination and stock demand posting
</commit_message>
<xml_diff>
--- a/TFP_Sprint_Board-11092023 (1).xlsx
+++ b/TFP_Sprint_Board-11092023 (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah.nadim\Desktop\Nadim_Work\UiPath\Central Ordering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315293EC-B755-47DA-87B1-1036A817CDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30C977D-C1D5-4943-B7F8-2B624DCE49C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="10" activeTab="12" xr2:uid="{A4006B41-6FF4-47DD-AE94-8399D65B0D9D}"/>
+    <workbookView xWindow="-20610" yWindow="-60" windowWidth="20730" windowHeight="11040" firstSheet="10" activeTab="12" xr2:uid="{A4006B41-6FF4-47DD-AE94-8399D65B0D9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 21 10.10 - 21.10" sheetId="2" state="hidden" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="191">
   <si>
     <t> </t>
   </si>
@@ -1606,28 +1606,43 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Development Done, Pending for UAT </t>
-  </si>
-  <si>
     <t xml:space="preserve">BOT Installation on user computer done.User is checking with different files data to on LS System. </t>
   </si>
   <si>
-    <t xml:space="preserve"> In progress with LS data. Exception raised on some data which was not handled during  development. Finishing those. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Development done , Fixing some exceptions raised at User End </t>
-  </si>
-  <si>
     <t>BOT Installation on user computer done.</t>
   </si>
   <si>
-    <t>After Exception handled from My end UAT Sign OFF will Done</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Bot Installation done.</t>
+  </si>
+  <si>
+    <t>Development Done, UAT Done, Signedoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development done , Fixing some exceptions raised at User End because of Change request. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Done, Exception Handling because of change request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done,  Gave User document which includes all information how to run the bot, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As per user request partial process was deployed, Posting to LS is not done yet. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development Done, But in this section when testing against UAT lots of exception occurs because UAT is not up to date.  </t>
+  </si>
+  <si>
+    <t>Integration to LS system done</t>
   </si>
 </sst>
 </file>
@@ -2210,6 +2225,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2218,9 +2236,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4550,8 +4565,8 @@
   </sheetPr>
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4767,7 +4782,7 @@
       <c r="I7" s="50"/>
       <c r="J7" s="50"/>
     </row>
-    <row r="8" spans="1:21" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>7</v>
       </c>
@@ -4867,12 +4882,12 @@
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
       <c r="F12" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" s="74" t="s">
         <v>176</v>
       </c>
-      <c r="H12" s="109">
+      <c r="H12" s="110">
         <v>45204</v>
       </c>
       <c r="I12" s="50"/>
@@ -4889,12 +4904,12 @@
       <c r="D13" s="100"/>
       <c r="E13" s="100"/>
       <c r="F13" s="100" t="s">
-        <v>178</v>
-      </c>
-      <c r="G13" s="112" t="s">
-        <v>182</v>
-      </c>
-      <c r="H13" s="110"/>
+        <v>181</v>
+      </c>
+      <c r="G13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="111"/>
       <c r="I13" s="102"/>
       <c r="J13" s="98"/>
     </row>
@@ -4909,12 +4924,12 @@
       <c r="D14" s="106"/>
       <c r="E14" s="106"/>
       <c r="F14" s="106" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G14" s="101" t="s">
-        <v>179</v>
-      </c>
-      <c r="H14" s="110"/>
+        <v>178</v>
+      </c>
+      <c r="H14" s="111"/>
       <c r="I14" s="107"/>
       <c r="J14" s="104"/>
     </row>
@@ -4932,7 +4947,7 @@
         <v>183</v>
       </c>
       <c r="G15" s="94"/>
-      <c r="H15" s="110"/>
+      <c r="H15" s="111"/>
       <c r="I15" s="95"/>
       <c r="J15" s="91"/>
     </row>
@@ -4947,12 +4962,12 @@
       <c r="D16" s="93"/>
       <c r="E16" s="93"/>
       <c r="F16" s="93" t="s">
+        <v>189</v>
+      </c>
+      <c r="G16" s="94" t="s">
         <v>180</v>
       </c>
-      <c r="G16" s="94" t="s">
-        <v>185</v>
-      </c>
-      <c r="H16" s="111"/>
+      <c r="H16" s="112"/>
       <c r="I16" s="95"/>
       <c r="J16" s="91"/>
     </row>
@@ -4968,7 +4983,9 @@
       </c>
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
+      <c r="F17" s="46" t="s">
+        <v>190</v>
+      </c>
       <c r="G17" s="74"/>
       <c r="H17" s="50">
         <v>45209</v>
@@ -5030,7 +5047,9 @@
       </c>
       <c r="D20" s="46"/>
       <c r="E20" s="46"/>
-      <c r="F20" s="60"/>
+      <c r="F20" s="60" t="s">
+        <v>185</v>
+      </c>
       <c r="G20" s="74"/>
       <c r="H20" s="78">
         <v>45211</v>
@@ -5051,7 +5070,7 @@
       <c r="D21" s="46"/>
       <c r="E21" s="46"/>
       <c r="F21" s="46" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G21" s="74"/>
       <c r="H21" s="50">
@@ -5092,7 +5111,9 @@
       </c>
       <c r="D23" s="52"/>
       <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
+      <c r="F23" s="52" t="s">
+        <v>188</v>
+      </c>
       <c r="G23" s="72"/>
       <c r="H23" s="50">
         <v>45219</v>
@@ -5112,7 +5133,9 @@
       </c>
       <c r="D24" s="46"/>
       <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
+      <c r="F24" s="46" t="s">
+        <v>187</v>
+      </c>
       <c r="G24" s="74"/>
       <c r="H24" s="50">
         <v>45220</v>

</xml_diff>

<commit_message>
VG Excel Combination Part 1 done
</commit_message>
<xml_diff>
--- a/TFP_Sprint_Board-11092023 (1).xlsx
+++ b/TFP_Sprint_Board-11092023 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah.nadim\Desktop\Nadim_Work\UiPath\Central Ordering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30C977D-C1D5-4943-B7F8-2B624DCE49C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3CFB33-F449-4D43-A1A8-B8CF9338ECDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-60" windowWidth="20730" windowHeight="11040" firstSheet="10" activeTab="12" xr2:uid="{A4006B41-6FF4-47DD-AE94-8399D65B0D9D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="10" activeTab="12" xr2:uid="{A4006B41-6FF4-47DD-AE94-8399D65B0D9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 21 10.10 - 21.10" sheetId="2" state="hidden" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="191">
   <si>
     <t> </t>
   </si>
@@ -1606,43 +1606,43 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">BOT Installation on user computer done.User is checking with different files data to on LS System. </t>
-  </si>
-  <si>
-    <t>BOT Installation on user computer done.</t>
-  </si>
-  <si>
-    <t>Bot Installation done.</t>
-  </si>
-  <si>
     <t>Development Done, UAT Done, Signedoff</t>
   </si>
   <si>
-    <t xml:space="preserve">Development done , Fixing some exceptions raised at User End because of Change request. </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Done, Exception Handling because of change request.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Partial </t>
   </si>
   <si>
     <t xml:space="preserve">Full </t>
   </si>
   <si>
-    <t xml:space="preserve">Done,  Gave User document which includes all information how to run the bot, </t>
-  </si>
-  <si>
     <t xml:space="preserve">As per user request partial process was deployed, Posting to LS is not done yet. </t>
   </si>
   <si>
-    <t xml:space="preserve">Development Done, But in this section when testing against UAT lots of exception occurs because UAT is not up to date.  </t>
-  </si>
-  <si>
     <t>Integration to LS system done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development done. UAT IN PROGRESS </t>
+  </si>
+  <si>
+    <t>Development Done,UAT DONE</t>
+  </si>
+  <si>
+    <t>ONLY SUBPROCESS 2</t>
+  </si>
+  <si>
+    <t>Done,  Gave User document which includes all information how to run the bot, Instructions and Prerequisits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOT Installation on user computer done. And Started Using on Prod Environment. </t>
+  </si>
+  <si>
+    <t>BOT Installation on user computer done.User is checking  after changed request changes are done.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bot Installation done. </t>
   </si>
 </sst>
 </file>
@@ -4565,8 +4565,8 @@
   </sheetPr>
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4904,10 +4904,10 @@
       <c r="D13" s="100"/>
       <c r="E13" s="100"/>
       <c r="F13" s="100" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G13" s="109" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="H13" s="111"/>
       <c r="I13" s="102"/>
@@ -4924,10 +4924,10 @@
       <c r="D14" s="106"/>
       <c r="E14" s="106"/>
       <c r="F14" s="106" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G14" s="101" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="H14" s="111"/>
       <c r="I14" s="107"/>
@@ -4944,7 +4944,7 @@
       <c r="D15" s="93"/>
       <c r="E15" s="93"/>
       <c r="F15" s="93" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G15" s="94"/>
       <c r="H15" s="111"/>
@@ -4962,10 +4962,10 @@
       <c r="D16" s="93"/>
       <c r="E16" s="93"/>
       <c r="F16" s="93" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G16" s="94" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="H16" s="112"/>
       <c r="I16" s="95"/>
@@ -4984,7 +4984,7 @@
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
       <c r="F17" s="46" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="G17" s="74"/>
       <c r="H17" s="50">
@@ -5026,7 +5026,7 @@
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G19" s="75"/>
       <c r="H19" s="97">
@@ -5048,7 +5048,7 @@
       <c r="D20" s="46"/>
       <c r="E20" s="46"/>
       <c r="F20" s="60" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G20" s="74"/>
       <c r="H20" s="78">
@@ -5070,9 +5070,11 @@
       <c r="D21" s="46"/>
       <c r="E21" s="46"/>
       <c r="F21" s="46" t="s">
-        <v>186</v>
-      </c>
-      <c r="G21" s="74"/>
+        <v>181</v>
+      </c>
+      <c r="G21" s="74" t="s">
+        <v>179</v>
+      </c>
       <c r="H21" s="50">
         <v>45216</v>
       </c>
@@ -5112,7 +5114,7 @@
       <c r="D23" s="52"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G23" s="72"/>
       <c r="H23" s="50">

</xml_diff>

<commit_message>
central ordering with Excel Manipulation
</commit_message>
<xml_diff>
--- a/TFP_Sprint_Board-11092023 (1).xlsx
+++ b/TFP_Sprint_Board-11092023 (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah.nadim\Desktop\Nadim_Work\UiPath\Central Ordering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3CFB33-F449-4D43-A1A8-B8CF9338ECDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B834F3E-BF8A-4896-B840-9FF9829B464A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="10" activeTab="12" xr2:uid="{A4006B41-6FF4-47DD-AE94-8399D65B0D9D}"/>
+    <workbookView xWindow="-20610" yWindow="-60" windowWidth="20730" windowHeight="11040" firstSheet="11" activeTab="13" xr2:uid="{A4006B41-6FF4-47DD-AE94-8399D65B0D9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 21 10.10 - 21.10" sheetId="2" state="hidden" r:id="rId1"/>
@@ -20,114 +20,115 @@
     <sheet name="Petty cash reminder" sheetId="9" r:id="rId5"/>
     <sheet name="Non Trade - Utilities - Gas" sheetId="8" r:id="rId6"/>
     <sheet name="Non Trade - Utilities - IDK" sheetId="16" r:id="rId7"/>
-    <sheet name="Non Trade - Utilities - Time" sheetId="17" r:id="rId8"/>
-    <sheet name="Non Trade - Utilities - TNB" sheetId="10" r:id="rId9"/>
-    <sheet name="Non Trade - Utilities - Celcom" sheetId="11" r:id="rId10"/>
-    <sheet name="Non Trade - Utilities - TM" sheetId="13" r:id="rId11"/>
-    <sheet name="Non Trade - Utilities - Syabas" sheetId="15" r:id="rId12"/>
-    <sheet name="Central Ordering " sheetId="18" r:id="rId13"/>
+    <sheet name="Central Ordering " sheetId="18" r:id="rId8"/>
+    <sheet name="Non Trade - Utilities - Time" sheetId="17" r:id="rId9"/>
+    <sheet name="Non Trade - Utilities - TNB" sheetId="10" r:id="rId10"/>
+    <sheet name="Non Trade - Utilities - Celcom" sheetId="11" r:id="rId11"/>
+    <sheet name="Non Trade - Utilities - TM" sheetId="13" r:id="rId12"/>
+    <sheet name="Non Trade - Utilities - Syabas" sheetId="15" r:id="rId13"/>
+    <sheet name="Price Matching" sheetId="19" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_3BBA7658_7877_46B6_942F_25D11FB44E32_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_3CC5409A_C016_497F_9C2F_9F1DF0FF1E46_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_59D37F8E_1ADB_40C6_826D_6E0074D60B93_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_7B71EA5E_2CCD_4C4D_9A6B_2A7C88088000_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_7F4C36EE_9459_40AE_B958_CF7B91168615_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_8FC86742_3CD8_4BEA_9CD4_811B7948F5D7_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_A5FCDD78_7C72_4CF1_917B_862F7A7497E2_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_BFC50948_4173_4DDA_BCDF_E2CF54FD8FE6_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_C316EC84_A196_4549_A6CD_59342942EBA0_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
     <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="2" hidden="1">' CR-OTC'!#REF!</definedName>
     <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="1" hidden="1">' tracking Consignment '!#REF!</definedName>
     <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="3" hidden="1">' tracking NT PO Approval'!#REF!</definedName>
-    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
+    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - Celcom'!#REF!</definedName>
     <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="5" hidden="1">'Non Trade - Utilities - Gas'!#REF!</definedName>
     <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="6" hidden="1">'Non Trade - Utilities - IDK'!#REF!</definedName>
-    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
-    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="7" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
-    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="10" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
-    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
+    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="12" hidden="1">'Non Trade - Utilities - Syabas'!#REF!</definedName>
+    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="8" hidden="1">'Non Trade - Utilities - Time'!#REF!</definedName>
+    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="11" hidden="1">'Non Trade - Utilities - TM'!#REF!</definedName>
+    <definedName name="Z_D500F207_6176_4947_B32A_61D483D43DA7_.wvu.Cols" localSheetId="9" hidden="1">'Non Trade - Utilities - TNB'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -150,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="199">
   <si>
     <t> </t>
   </si>
@@ -1612,15 +1613,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Partial </t>
-  </si>
-  <si>
     <t xml:space="preserve">Full </t>
   </si>
   <si>
-    <t xml:space="preserve">As per user request partial process was deployed, Posting to LS is not done yet. </t>
-  </si>
-  <si>
     <t>Integration to LS system done</t>
   </si>
   <si>
@@ -1630,9 +1625,6 @@
     <t>Development Done,UAT DONE</t>
   </si>
   <si>
-    <t>ONLY SUBPROCESS 2</t>
-  </si>
-  <si>
     <t>Done,  Gave User document which includes all information how to run the bot, Instructions and Prerequisits</t>
   </si>
   <si>
@@ -1643,6 +1635,99 @@
   </si>
   <si>
     <t xml:space="preserve">Bot Installation done. </t>
+  </si>
+  <si>
+    <t>Some issue came up when doing Production process run. Solving it when any problem arises , Such as searching ITEM is not present or taking too much time to respond. Pop up like Working on it, Searching is slow .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> process is deployed.</t>
+  </si>
+  <si>
+    <t>Tan Joo Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	14/11/2023</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Development Sub Process 1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prepare file for Merchandising Feedback</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Development Sub Process 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Received Feedback from Merchandising Team </t>
+    </r>
+  </si>
+  <si>
+    <t>Create a priceing file using previous month's file template which has all the new prices of competitor</t>
+  </si>
+  <si>
+    <t>After receiving the excel file which is verified by the merchadinsing team Update the price with appropriate conditions.</t>
+  </si>
+  <si>
+    <t>email Price Match Result, and update the file with adding in last month's data .</t>
+  </si>
+  <si>
+    <t>1. Need to seat with the user to see the process &amp; understand the process workings , also for test data. 2. Queries that I have after seeing the video and PDD.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Development Sub Process 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Emailing the Excel and add new data .</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1652,7 +1737,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1777,8 +1862,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1869,6 +1961,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -1949,7 +2047,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2236,6 +2334,31 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3065,6 +3188,504 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480BA2A7-8C26-4C45-BC92-1F3AC69A4817}">
+  <dimension ref="A1:U20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" style="48" customWidth="1"/>
+    <col min="2" max="3" width="33.42578125" style="49" customWidth="1"/>
+    <col min="4" max="4" width="38" style="48" customWidth="1"/>
+    <col min="5" max="5" width="0.140625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="48" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="76" customWidth="1"/>
+    <col min="8" max="9" width="31.42578125" style="43" customWidth="1"/>
+    <col min="10" max="10" width="42.85546875" style="43" customWidth="1"/>
+    <col min="11" max="18" width="8.5703125" style="43"/>
+    <col min="19" max="19" width="26.42578125" style="43" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.5703125" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="44">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="74"/>
+      <c r="H2" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="S2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="44">
+        <v>2</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="74"/>
+      <c r="H3" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="44">
+        <v>3</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="74"/>
+      <c r="H4" s="50">
+        <v>45093</v>
+      </c>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50">
+        <v>45093</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>4</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="74"/>
+      <c r="H5" s="50">
+        <v>45104</v>
+      </c>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50">
+        <v>45104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="44">
+        <v>5</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="74"/>
+      <c r="H6" s="50">
+        <v>45111</v>
+      </c>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50">
+        <v>45111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="44">
+        <v>6</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="74"/>
+      <c r="H7" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50">
+        <v>45119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="44">
+        <v>7</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="72" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="I8" s="50"/>
+      <c r="J8" s="44"/>
+    </row>
+    <row r="9" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="44">
+        <v>8</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="50">
+        <v>45145</v>
+      </c>
+      <c r="I9" s="50"/>
+      <c r="J9" s="44"/>
+    </row>
+    <row r="10" spans="1:21" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="44">
+        <v>7</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" s="74"/>
+      <c r="H10" s="50">
+        <v>45146</v>
+      </c>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+    </row>
+    <row r="11" spans="1:21" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="44">
+        <v>8</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11" s="74"/>
+      <c r="H11" s="50">
+        <v>45146</v>
+      </c>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="44">
+        <v>9</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="50">
+        <v>45168</v>
+      </c>
+      <c r="I12" s="50">
+        <v>45163</v>
+      </c>
+      <c r="J12" s="44"/>
+    </row>
+    <row r="13" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="44">
+        <v>10</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50">
+        <v>45166</v>
+      </c>
+      <c r="J13" s="44"/>
+    </row>
+    <row r="14" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="44">
+        <v>11</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="62"/>
+    </row>
+    <row r="15" spans="1:21" s="61" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="58">
+        <v>12</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="78">
+        <v>45174</v>
+      </c>
+      <c r="I15" s="78">
+        <v>45168</v>
+      </c>
+      <c r="J15" s="58"/>
+    </row>
+    <row r="16" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="44">
+        <v>13</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="71">
+        <v>45175</v>
+      </c>
+      <c r="I16" s="71">
+        <v>45170</v>
+      </c>
+      <c r="J16" s="63"/>
+    </row>
+    <row r="17" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="44">
+        <v>14</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="50">
+        <v>45180</v>
+      </c>
+      <c r="I17" s="50">
+        <v>45173</v>
+      </c>
+      <c r="J17" s="44"/>
+    </row>
+    <row r="18" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="44">
+        <v>15</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50">
+        <v>45174</v>
+      </c>
+      <c r="J18" s="44"/>
+    </row>
+    <row r="19" spans="1:10" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="44">
+        <v>15</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="50">
+        <v>45182</v>
+      </c>
+      <c r="I19" s="50">
+        <v>45174</v>
+      </c>
+      <c r="J19" s="44"/>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="44">
+        <v>16</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="50">
+        <v>45183</v>
+      </c>
+      <c r="I20" s="50">
+        <v>45175</v>
+      </c>
+      <c r="J20" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728B9999-4289-4B51-931A-BD6934AB5950}">
   <dimension ref="A1:U20"/>
   <sheetViews>
@@ -3562,7 +4183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25C2B62-4F28-4464-A6C3-F4C1BB6CCC1C}">
   <dimension ref="A1:U20"/>
   <sheetViews>
@@ -4060,7 +4681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5682CE-AA3D-4C48-8B9A-7E4CC00BB4A1}">
   <dimension ref="A1:U20"/>
   <sheetViews>
@@ -4558,34 +5179,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3559751-38E2-4AE9-9E91-22F911517689}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:U24"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7526ED7-1432-46BD-9C4F-926961A2B511}">
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4" style="48" customWidth="1"/>
-    <col min="2" max="3" width="33.42578125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="38" style="48" customWidth="1"/>
-    <col min="5" max="5" width="0.140625" style="48" customWidth="1"/>
-    <col min="6" max="6" width="40" style="48" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="76" customWidth="1"/>
-    <col min="8" max="9" width="31.42578125" style="43" customWidth="1"/>
-    <col min="10" max="10" width="42.85546875" style="43" customWidth="1"/>
-    <col min="11" max="18" width="8.5703125" style="43"/>
-    <col min="19" max="19" width="26.42578125" style="43" customWidth="1"/>
-    <col min="20" max="20" width="17.28515625" style="43" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.5703125" style="43"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>56</v>
       </c>
@@ -4617,7 +5221,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="44">
         <v>1</v>
       </c>
@@ -4628,7 +5232,7 @@
         <v>102</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="E2" s="46"/>
       <c r="F2" s="70" t="s">
@@ -4636,25 +5240,16 @@
       </c>
       <c r="G2" s="74"/>
       <c r="H2" s="44" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="I2" s="50">
-        <v>45180</v>
+        <v>45244</v>
       </c>
       <c r="J2" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="S2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="44">
         <v>2</v>
       </c>
@@ -4665,7 +5260,7 @@
         <v>114</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="E3" s="46"/>
       <c r="F3" s="70" t="s">
@@ -4673,16 +5268,16 @@
       </c>
       <c r="G3" s="74"/>
       <c r="H3" s="44" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="I3" s="50">
-        <v>45173</v>
+        <v>45244</v>
       </c>
       <c r="J3" s="44" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="44">
         <v>3</v>
       </c>
@@ -4693,7 +5288,7 @@
         <v>115</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="70" t="s">
@@ -4701,14 +5296,14 @@
       </c>
       <c r="G4" s="74"/>
       <c r="H4" s="44" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I4" s="50">
-        <v>45173</v>
+        <v>45244</v>
       </c>
       <c r="J4" s="50"/>
     </row>
-    <row r="5" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="44">
         <v>4</v>
       </c>
@@ -4719,7 +5314,7 @@
         <v>116</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="E5" s="46"/>
       <c r="F5" s="70" t="s">
@@ -4727,14 +5322,14 @@
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="44" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I5" s="50">
-        <v>45173</v>
+        <v>45244</v>
       </c>
       <c r="J5" s="50"/>
     </row>
-    <row r="6" spans="1:21" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="44">
         <v>5</v>
       </c>
@@ -4745,7 +5340,7 @@
         <v>103</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="70" t="s">
@@ -4753,14 +5348,14 @@
       </c>
       <c r="G6" s="74"/>
       <c r="H6" s="44" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="I6" s="50">
-        <v>45173</v>
+        <v>45244</v>
       </c>
       <c r="J6" s="50"/>
     </row>
-    <row r="7" spans="1:21" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A7" s="44">
         <v>6</v>
       </c>
@@ -4773,16 +5368,16 @@
       <c r="D7" s="46"/>
       <c r="E7" s="46"/>
       <c r="F7" s="70" t="s">
-        <v>168</v>
+        <v>81</v>
       </c>
       <c r="G7" s="74"/>
-      <c r="H7" s="50" t="s">
-        <v>166</v>
+      <c r="H7" s="44" t="s">
+        <v>191</v>
       </c>
       <c r="I7" s="50"/>
       <c r="J7" s="50"/>
     </row>
-    <row r="8" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>7</v>
       </c>
@@ -4800,13 +5395,13 @@
       <c r="G8" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="44" t="s">
         <v>166</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="44"/>
     </row>
-    <row r="9" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="44">
         <v>8</v>
       </c>
@@ -4818,14 +5413,13 @@
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
-      <c r="F9" s="46" t="s">
-        <v>155</v>
-      </c>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
       <c r="H9" s="50"/>
       <c r="I9" s="50"/>
       <c r="J9" s="44"/>
     </row>
-    <row r="10" spans="1:21" s="90" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="85">
         <v>7</v>
       </c>
@@ -4837,17 +5431,13 @@
       </c>
       <c r="D10" s="87"/>
       <c r="E10" s="87"/>
-      <c r="F10" s="87" t="s">
-        <v>81</v>
-      </c>
+      <c r="F10" s="87"/>
       <c r="G10" s="88"/>
-      <c r="H10" s="89">
-        <v>45183</v>
-      </c>
+      <c r="H10" s="89"/>
       <c r="I10" s="89"/>
       <c r="J10" s="89"/>
     </row>
-    <row r="11" spans="1:21" s="84" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="79">
         <v>8</v>
       </c>
@@ -4859,17 +5449,13 @@
       </c>
       <c r="D11" s="81"/>
       <c r="E11" s="81"/>
-      <c r="F11" s="81" t="s">
-        <v>155</v>
-      </c>
+      <c r="F11" s="81"/>
       <c r="G11" s="82"/>
-      <c r="H11" s="83">
-        <v>45184</v>
-      </c>
+      <c r="H11" s="83"/>
       <c r="I11" s="83"/>
       <c r="J11" s="83"/>
     </row>
-    <row r="12" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="44">
         <v>9</v>
       </c>
@@ -4881,277 +5467,318 @@
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
-      <c r="F12" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" s="74" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="110">
-        <v>45204</v>
-      </c>
+      <c r="F12" s="46"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="110"/>
       <c r="I12" s="50"/>
       <c r="J12" s="44"/>
     </row>
-    <row r="13" spans="1:21" s="103" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="98"/>
-      <c r="B13" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="99" t="s">
-        <v>175</v>
-      </c>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100" t="s">
-        <v>178</v>
-      </c>
-      <c r="G13" s="109" t="s">
-        <v>188</v>
-      </c>
+    <row r="13" spans="1:10" s="119" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="113"/>
+      <c r="B13" s="114" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="114" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="116"/>
       <c r="H13" s="111"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="98"/>
-    </row>
-    <row r="14" spans="1:21" s="108" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" s="104"/>
-      <c r="B14" s="105" t="s">
-        <v>170</v>
-      </c>
-      <c r="C14" s="105" t="s">
-        <v>177</v>
-      </c>
-      <c r="D14" s="106"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106" t="s">
-        <v>184</v>
-      </c>
-      <c r="G14" s="101" t="s">
-        <v>189</v>
-      </c>
+      <c r="I13" s="117"/>
+      <c r="J13" s="113"/>
+    </row>
+    <row r="14" spans="1:10" s="119" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="113"/>
+      <c r="B14" s="114" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="114" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115" t="s">
+        <v>179</v>
+      </c>
+      <c r="G14" s="118"/>
       <c r="H14" s="111"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="104"/>
-    </row>
-    <row r="15" spans="1:21" s="96" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="91"/>
-      <c r="B15" s="92" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15" s="92" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93" t="s">
+      <c r="I14" s="117"/>
+      <c r="J14" s="113"/>
+    </row>
+    <row r="15" spans="1:10" s="119" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="113"/>
+      <c r="B15" s="114" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" s="114" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="118" t="s">
         <v>179</v>
       </c>
-      <c r="G15" s="94"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="91"/>
-    </row>
-    <row r="16" spans="1:21" s="96" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="91"/>
-      <c r="B16" s="92" t="s">
-        <v>172</v>
-      </c>
-      <c r="C16" s="92" t="s">
-        <v>174</v>
-      </c>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93" t="s">
-        <v>185</v>
-      </c>
-      <c r="G16" s="94" t="s">
-        <v>190</v>
-      </c>
-      <c r="H16" s="112"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="91"/>
-    </row>
-    <row r="17" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H15" s="112"/>
+      <c r="I15" s="117"/>
+      <c r="J15" s="113"/>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="44">
+        <v>10</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="44"/>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="44">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
-      <c r="F17" s="46" t="s">
-        <v>183</v>
-      </c>
+      <c r="F17" s="46"/>
       <c r="G17" s="74"/>
-      <c r="H17" s="50">
-        <v>45209</v>
-      </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="44"/>
-    </row>
-    <row r="18" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
-        <v>11</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="50">
-        <v>45209</v>
-      </c>
-      <c r="I18" s="77"/>
-      <c r="J18" s="62"/>
-    </row>
-    <row r="19" spans="1:10" s="61" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="58">
+      <c r="H17" s="50"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="62"/>
+    </row>
+    <row r="18" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+      <c r="A18" s="58">
         <v>12</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B18" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C18" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60" t="s">
-        <v>186</v>
-      </c>
-      <c r="G19" s="75"/>
-      <c r="H19" s="97">
-        <v>45210</v>
-      </c>
-      <c r="I19" s="78"/>
-      <c r="J19" s="58"/>
-    </row>
-    <row r="20" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="58"/>
+    </row>
+    <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="44">
+        <v>13</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="63"/>
+    </row>
+    <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="44">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D20" s="46"/>
       <c r="E20" s="46"/>
-      <c r="F20" s="60" t="s">
-        <v>180</v>
-      </c>
-      <c r="G20" s="74"/>
-      <c r="H20" s="78">
-        <v>45211</v>
-      </c>
-      <c r="I20" s="71"/>
-      <c r="J20" s="63"/>
-    </row>
-    <row r="21" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F20" s="46"/>
+      <c r="G20" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="44"/>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="44">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D21" s="46"/>
       <c r="E21" s="46"/>
-      <c r="F21" s="46" t="s">
-        <v>181</v>
-      </c>
-      <c r="G21" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="H21" s="50">
-        <v>45216</v>
-      </c>
+      <c r="F21" s="46"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="50"/>
       <c r="I21" s="50"/>
       <c r="J21" s="44"/>
     </row>
-    <row r="22" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="44">
         <v>15</v>
       </c>
-      <c r="B22" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="50">
-        <v>45217</v>
-      </c>
+      <c r="B22" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="50"/>
       <c r="I22" s="50"/>
       <c r="J22" s="44"/>
     </row>
-    <row r="23" spans="1:10" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="44">
-        <v>15</v>
-      </c>
-      <c r="B23" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52" t="s">
-        <v>182</v>
-      </c>
-      <c r="G23" s="72"/>
-      <c r="H23" s="50">
-        <v>45219</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="50"/>
       <c r="I23" s="50"/>
       <c r="J23" s="44"/>
     </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="44">
-        <v>16</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="G24" s="74"/>
-      <c r="H24" s="50">
-        <v>45220</v>
-      </c>
-      <c r="I24" s="50"/>
-      <c r="J24" s="44"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="121" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" s="120"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="120"/>
+      <c r="F29" s="120"/>
+      <c r="G29" s="120"/>
+      <c r="H29" s="120"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="120"/>
+      <c r="C30" s="120"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="120"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="120"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="120"/>
+      <c r="C31" s="120"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="120"/>
+      <c r="G31" s="120"/>
+      <c r="H31" s="120"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="120"/>
+      <c r="C32" s="120"/>
+      <c r="D32" s="120"/>
+      <c r="E32" s="120"/>
+      <c r="F32" s="120"/>
+      <c r="G32" s="120"/>
+      <c r="H32" s="120"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="120"/>
+      <c r="C33" s="120"/>
+      <c r="D33" s="120"/>
+      <c r="E33" s="120"/>
+      <c r="F33" s="120"/>
+      <c r="G33" s="120"/>
+      <c r="H33" s="120"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="120"/>
+      <c r="C34" s="120"/>
+      <c r="D34" s="120"/>
+      <c r="E34" s="120"/>
+      <c r="F34" s="120"/>
+      <c r="G34" s="120"/>
+      <c r="H34" s="120"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="120"/>
+      <c r="C35" s="120"/>
+      <c r="D35" s="120"/>
+      <c r="E35" s="120"/>
+      <c r="F35" s="120"/>
+      <c r="G35" s="120"/>
+      <c r="H35" s="120"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="120"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="120"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="120"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="120"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="120"/>
+      <c r="F37" s="120"/>
+      <c r="G37" s="120"/>
+      <c r="H37" s="120"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="120"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="120"/>
+      <c r="F38" s="120"/>
+      <c r="G38" s="120"/>
+      <c r="H38" s="120"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="120"/>
+      <c r="C39" s="120"/>
+      <c r="D39" s="120"/>
+      <c r="E39" s="120"/>
+      <c r="F39" s="120"/>
+      <c r="G39" s="120"/>
+      <c r="H39" s="120"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H12:H16"/>
+  <mergeCells count="2">
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="B29:H39"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="50" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7284,6 +7911,601 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3559751-38E2-4AE9-9E91-22F911517689}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:U24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="A1:J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" style="48" customWidth="1"/>
+    <col min="2" max="3" width="33.42578125" style="49" customWidth="1"/>
+    <col min="4" max="4" width="38" style="48" customWidth="1"/>
+    <col min="5" max="5" width="0.140625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="40" style="48" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="76" customWidth="1"/>
+    <col min="8" max="9" width="31.42578125" style="43" customWidth="1"/>
+    <col min="10" max="10" width="42.85546875" style="43" customWidth="1"/>
+    <col min="11" max="18" width="8.5703125" style="43"/>
+    <col min="19" max="19" width="26.42578125" style="43" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.5703125" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="44">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="46"/>
+      <c r="F2" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="74"/>
+      <c r="H2" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="50">
+        <v>45180</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="S2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="44">
+        <v>2</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="74"/>
+      <c r="H3" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="50">
+        <v>45173</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="44">
+        <v>3</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="46"/>
+      <c r="F4" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="74"/>
+      <c r="H4" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="I4" s="50">
+        <v>45173</v>
+      </c>
+      <c r="J4" s="50"/>
+    </row>
+    <row r="5" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>4</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="46"/>
+      <c r="F5" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="74"/>
+      <c r="H5" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" s="50">
+        <v>45173</v>
+      </c>
+      <c r="J5" s="50"/>
+    </row>
+    <row r="6" spans="1:21" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="44">
+        <v>5</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="74"/>
+      <c r="H6" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="50">
+        <v>45173</v>
+      </c>
+      <c r="J6" s="50"/>
+    </row>
+    <row r="7" spans="1:21" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="44">
+        <v>6</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="74"/>
+      <c r="H7" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+    </row>
+    <row r="8" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="44">
+        <v>7</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" s="50"/>
+      <c r="J8" s="44"/>
+    </row>
+    <row r="9" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="44">
+        <v>8</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="44"/>
+    </row>
+    <row r="10" spans="1:21" s="90" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="85">
+        <v>7</v>
+      </c>
+      <c r="B10" s="86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="86" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="88"/>
+      <c r="H10" s="89">
+        <v>45183</v>
+      </c>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+    </row>
+    <row r="11" spans="1:21" s="84" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="79">
+        <v>8</v>
+      </c>
+      <c r="B11" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" s="82"/>
+      <c r="H11" s="83">
+        <v>45184</v>
+      </c>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+    </row>
+    <row r="12" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="44">
+        <v>9</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="110">
+        <v>45204</v>
+      </c>
+      <c r="I12" s="50"/>
+      <c r="J12" s="44"/>
+    </row>
+    <row r="13" spans="1:21" s="103" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="98"/>
+      <c r="B13" s="99" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100" t="s">
+        <v>178</v>
+      </c>
+      <c r="G13" s="109" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" s="111"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="98"/>
+    </row>
+    <row r="14" spans="1:21" s="108" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="104"/>
+      <c r="B14" s="105" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="106"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="106" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="101" t="s">
+        <v>186</v>
+      </c>
+      <c r="H14" s="111"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="104"/>
+    </row>
+    <row r="15" spans="1:21" s="96" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="91"/>
+      <c r="B15" s="92" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="92" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93" t="s">
+        <v>179</v>
+      </c>
+      <c r="G15" s="94"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="91"/>
+    </row>
+    <row r="16" spans="1:21" s="96" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="91"/>
+      <c r="B16" s="92" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="92" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93" t="s">
+        <v>183</v>
+      </c>
+      <c r="G16" s="94" t="s">
+        <v>187</v>
+      </c>
+      <c r="H16" s="112"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="91"/>
+    </row>
+    <row r="17" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="44">
+        <v>10</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="G17" s="74"/>
+      <c r="H17" s="50">
+        <v>45209</v>
+      </c>
+      <c r="I17" s="50"/>
+      <c r="J17" s="44"/>
+    </row>
+    <row r="18" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44">
+        <v>11</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="50">
+        <v>45209</v>
+      </c>
+      <c r="I18" s="77"/>
+      <c r="J18" s="62"/>
+    </row>
+    <row r="19" spans="1:10" s="61" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="58">
+        <v>12</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="97">
+        <v>45210</v>
+      </c>
+      <c r="I19" s="78"/>
+      <c r="J19" s="58"/>
+    </row>
+    <row r="20" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="44">
+        <v>13</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="78">
+        <v>45211</v>
+      </c>
+      <c r="I20" s="71"/>
+      <c r="J20" s="63"/>
+    </row>
+    <row r="21" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="44">
+        <v>14</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="H21" s="50">
+        <v>45216</v>
+      </c>
+      <c r="I21" s="50"/>
+      <c r="J21" s="44"/>
+    </row>
+    <row r="22" spans="1:10" s="47" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="44">
+        <v>15</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="G22" s="74"/>
+      <c r="H22" s="50">
+        <v>45217</v>
+      </c>
+      <c r="I22" s="50"/>
+      <c r="J22" s="44"/>
+    </row>
+    <row r="23" spans="1:10" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="44">
+        <v>15</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="G23" s="72"/>
+      <c r="H23" s="50">
+        <v>45219</v>
+      </c>
+      <c r="I23" s="50"/>
+      <c r="J23" s="44"/>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="44">
+        <v>16</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="G24" s="74"/>
+      <c r="H24" s="50">
+        <v>45220</v>
+      </c>
+      <c r="I24" s="50"/>
+      <c r="J24" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H12:H16"/>
+  </mergeCells>
+  <phoneticPr fontId="17" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="50" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C06993-6FB5-4AB4-A397-2254CDAA5D11}">
   <dimension ref="A1:U20"/>
   <sheetViews>
@@ -7761,502 +8983,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480BA2A7-8C26-4C45-BC92-1F3AC69A4817}">
-  <dimension ref="A1:U20"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4" style="48" customWidth="1"/>
-    <col min="2" max="3" width="33.42578125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="38" style="48" customWidth="1"/>
-    <col min="5" max="5" width="0.140625" style="48" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="48" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="76" customWidth="1"/>
-    <col min="8" max="9" width="31.42578125" style="43" customWidth="1"/>
-    <col min="10" max="10" width="42.85546875" style="43" customWidth="1"/>
-    <col min="11" max="18" width="8.5703125" style="43"/>
-    <col min="19" max="19" width="26.42578125" style="43" customWidth="1"/>
-    <col min="20" max="20" width="17.28515625" style="43" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.5703125" style="43"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="44">
-        <v>1</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="S2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="44">
-        <v>2</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="44" t="s">
-        <v>140</v>
-      </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
-        <v>3</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="50">
-        <v>45093</v>
-      </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50">
-        <v>45093</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
-        <v>4</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="50">
-        <v>45104</v>
-      </c>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50">
-        <v>45104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="44">
-        <v>5</v>
-      </c>
-      <c r="B6" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="74"/>
-      <c r="H6" s="50">
-        <v>45111</v>
-      </c>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50">
-        <v>45111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="44">
-        <v>6</v>
-      </c>
-      <c r="B7" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="50" t="s">
-        <v>141</v>
-      </c>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50">
-        <v>45119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="44">
-        <v>7</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" s="72" t="s">
-        <v>159</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="I8" s="50"/>
-      <c r="J8" s="44"/>
-    </row>
-    <row r="9" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="44">
-        <v>8</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="H9" s="50">
-        <v>45145</v>
-      </c>
-      <c r="I9" s="50"/>
-      <c r="J9" s="44"/>
-    </row>
-    <row r="10" spans="1:21" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="44">
-        <v>7</v>
-      </c>
-      <c r="B10" s="51" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10" s="74"/>
-      <c r="H10" s="50">
-        <v>45146</v>
-      </c>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-    </row>
-    <row r="11" spans="1:21" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="44">
-        <v>8</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" s="74"/>
-      <c r="H11" s="50">
-        <v>45146</v>
-      </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-    </row>
-    <row r="12" spans="1:21" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="44">
-        <v>9</v>
-      </c>
-      <c r="B12" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="74" t="s">
-        <v>160</v>
-      </c>
-      <c r="H12" s="50">
-        <v>45168</v>
-      </c>
-      <c r="I12" s="50">
-        <v>45163</v>
-      </c>
-      <c r="J12" s="44"/>
-    </row>
-    <row r="13" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="44">
-        <v>10</v>
-      </c>
-      <c r="B13" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50">
-        <v>45166</v>
-      </c>
-      <c r="J13" s="44"/>
-    </row>
-    <row r="14" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
-        <v>11</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="62"/>
-    </row>
-    <row r="15" spans="1:21" s="61" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="58">
-        <v>12</v>
-      </c>
-      <c r="B15" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="78">
-        <v>45174</v>
-      </c>
-      <c r="I15" s="78">
-        <v>45168</v>
-      </c>
-      <c r="J15" s="58"/>
-    </row>
-    <row r="16" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
-        <v>13</v>
-      </c>
-      <c r="B16" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="71">
-        <v>45175</v>
-      </c>
-      <c r="I16" s="71">
-        <v>45170</v>
-      </c>
-      <c r="J16" s="63"/>
-    </row>
-    <row r="17" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="44">
-        <v>14</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="50">
-        <v>45180</v>
-      </c>
-      <c r="I17" s="50">
-        <v>45173</v>
-      </c>
-      <c r="J17" s="44"/>
-    </row>
-    <row r="18" spans="1:10" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
-        <v>15</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50">
-        <v>45174</v>
-      </c>
-      <c r="J18" s="44"/>
-    </row>
-    <row r="19" spans="1:10" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="44">
-        <v>15</v>
-      </c>
-      <c r="B19" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="50">
-        <v>45182</v>
-      </c>
-      <c r="I19" s="50">
-        <v>45174</v>
-      </c>
-      <c r="J19" s="44"/>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="44">
-        <v>16</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="50">
-        <v>45183</v>
-      </c>
-      <c r="I20" s="50">
-        <v>45175</v>
-      </c>
-      <c r="J20" s="44"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>